<commit_message>
edit sms message and add logo for noyan
</commit_message>
<xml_diff>
--- a/public/noyan.xlsx
+++ b/public/noyan.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -529,9 +529,55 @@
         <v/>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>سپهر</v>
+      </c>
+      <c r="B6" t="str">
+        <v>09362172533</v>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v>۱۴۰۴/۷/۹, ۱۷:۵۵:۳۲</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>سپهر</v>
+      </c>
+      <c r="B7" t="str">
+        <v>09362172533</v>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v>۱۴۰۴/۷/۹, ۱۷:۵۹:۱۰</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>